<commit_message>
what if analysis, forecasting
</commit_message>
<xml_diff>
--- a/advanced_data_analysis/analysis_add-ins.xlsx
+++ b/advanced_data_analysis/analysis_add-ins.xlsx
@@ -8,58 +8,72 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walka\MyGit\excel\advanced_data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C25001D-CA3C-4C76-ADD0-ED7D26A5C5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E252BC9-CA7E-483C-9EF5-E127C4E59B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{BF3C499C-4EE3-4442-B128-B0E678080ACC}"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="13224" firstSheet="3" activeTab="7" xr2:uid="{BF3C499C-4EE3-4442-B128-B0E678080ACC}"/>
   </bookViews>
   <sheets>
     <sheet name="Forecast_Original" sheetId="2" r:id="rId1"/>
     <sheet name="Forecast_Final" sheetId="4" r:id="rId2"/>
-    <sheet name="What-If_Analysis" sheetId="5" r:id="rId3"/>
+    <sheet name="Scenario Summary" sheetId="7" r:id="rId3"/>
+    <sheet name="Answer Report 1" sheetId="8" r:id="rId4"/>
+    <sheet name="Sensitivity Report 1" sheetId="9" r:id="rId5"/>
+    <sheet name="Limits Report 1" sheetId="10" r:id="rId6"/>
+    <sheet name="Answer Report 2" sheetId="11" r:id="rId7"/>
+    <sheet name="What-If_Analysis" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="base" localSheetId="2">'What-If_Analysis'!$C$3</definedName>
-    <definedName name="bonus" localSheetId="2">'What-If_Analysis'!$C$4</definedName>
-    <definedName name="raise" localSheetId="2">'What-If_Analysis'!$C$5</definedName>
-    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'What-If_Analysis'!$C$4</definedName>
-    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'What-If_Analysis'!$C$5</definedName>
-    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="2" hidden="1">0.25</definedName>
-    <definedName name="solver_rhs2" localSheetId="2" hidden="1">0.035</definedName>
-    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="TotalSalary">'What-If_Analysis'!$C$14</definedName>
-    <definedName name="Year0">'What-If_Analysis'!$C$9</definedName>
-    <definedName name="Year1">'What-If_Analysis'!$C$10</definedName>
-    <definedName name="Year2">'What-If_Analysis'!$C$11</definedName>
-    <definedName name="Year3">'What-If_Analysis'!$C$12</definedName>
-    <definedName name="Year4">'What-If_Analysis'!$C$13</definedName>
+    <definedName name="base" localSheetId="7">'What-If_Analysis'!$C$3</definedName>
+    <definedName name="bonus" localSheetId="7">'What-If_Analysis'!$C$4</definedName>
+    <definedName name="raise" localSheetId="7">'What-If_Analysis'!$C$5</definedName>
+    <definedName name="solver_adj" localSheetId="7" hidden="1">'What-If_Analysis'!$C$4:$C$5</definedName>
+    <definedName name="solver_cvg" localSheetId="7" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="7" hidden="1">'What-If_Analysis'!$C$4</definedName>
+    <definedName name="solver_lhs2" localSheetId="7" hidden="1">'What-If_Analysis'!$C$5</definedName>
+    <definedName name="solver_mip" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="7" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="7" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_nwt" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="7" hidden="1">'What-If_Analysis'!$C$14</definedName>
+    <definedName name="solver_pre" localSheetId="7" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="7" hidden="1">0.2</definedName>
+    <definedName name="solver_rhs2" localSheetId="7" hidden="1">0.05</definedName>
+    <definedName name="solver_rlx" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="7" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="7" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="7" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="7" hidden="1">640000</definedName>
+    <definedName name="solver_ver" localSheetId="7" hidden="1">3</definedName>
+    <definedName name="TotalSalary" localSheetId="7">'What-If_Analysis'!$C$14</definedName>
+    <definedName name="TotalSalary">#REF!</definedName>
+    <definedName name="Year0" localSheetId="7">'What-If_Analysis'!$C$9</definedName>
+    <definedName name="Year0">#REF!</definedName>
+    <definedName name="Year1" localSheetId="7">'What-If_Analysis'!$C$10</definedName>
+    <definedName name="Year1">#REF!</definedName>
+    <definedName name="Year2" localSheetId="7">'What-If_Analysis'!$C$11</definedName>
+    <definedName name="Year2">#REF!</definedName>
+    <definedName name="Year3" localSheetId="7">'What-If_Analysis'!$C$12</definedName>
+    <definedName name="Year3">#REF!</definedName>
+    <definedName name="Year4" localSheetId="7">'What-If_Analysis'!$C$13</definedName>
+    <definedName name="Year4">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -80,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -130,7 +144,214 @@
     <t>Total</t>
   </si>
   <si>
-    <t xml:space="preserve">Job </t>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>Result Cells</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>bonus</t>
+  </si>
+  <si>
+    <t>raise</t>
+  </si>
+  <si>
+    <t>Year0</t>
+  </si>
+  <si>
+    <t>Year1</t>
+  </si>
+  <si>
+    <t>Year2</t>
+  </si>
+  <si>
+    <t>Year3</t>
+  </si>
+  <si>
+    <t>Year4</t>
+  </si>
+  <si>
+    <t>TotalSalary</t>
+  </si>
+  <si>
+    <t>Created by Raph Adam on 03 26 2025</t>
+  </si>
+  <si>
+    <t>Scenario Summary</t>
+  </si>
+  <si>
+    <t>Changing Cells:</t>
+  </si>
+  <si>
+    <t>Current Values:</t>
+  </si>
+  <si>
+    <t>Result Cells:</t>
+  </si>
+  <si>
+    <t>Notes:  Current Values column represents values of changing cells at</t>
+  </si>
+  <si>
+    <t>time Scenario Summary Report was created.  Changing cells for each</t>
+  </si>
+  <si>
+    <t>scenario are highlighted in gray.</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Answer Report</t>
+  </si>
+  <si>
+    <t>Worksheet: [analysis_add-ins.xlsx]What-If_Analysis</t>
+  </si>
+  <si>
+    <t>Report Created: Mar 26, 2025 2:37:21 PM</t>
+  </si>
+  <si>
+    <t>Result: Solver found a solution.  All Constraints and optimality conditions are satisfied.</t>
+  </si>
+  <si>
+    <t>Solver Engine</t>
+  </si>
+  <si>
+    <t>Engine: GRG Nonlinear</t>
+  </si>
+  <si>
+    <t>Solution Time: 0.093 Seconds.</t>
+  </si>
+  <si>
+    <t>Iterations: 0 Subproblems: 0</t>
+  </si>
+  <si>
+    <t>Solver Options</t>
+  </si>
+  <si>
+    <t>Max Time Unlimited,  Iterations Unlimited, Precision 0.000001, Use Automatic Scaling</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Convergence 0.0001, Population Size 100, Random Seed 0, Derivatives Forward, Require Bounds</t>
+  </si>
+  <si>
+    <t>Max Subproblems Unlimited, Max Integer Sols Unlimited, Integer Tolerance 1%, Assume NonNegative</t>
+  </si>
+  <si>
+    <t>Objective Cell (Value Of)</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Original Value</t>
+  </si>
+  <si>
+    <t>Final Value</t>
+  </si>
+  <si>
+    <t>Variable Cells</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>Cell Value</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Slack</t>
+  </si>
+  <si>
+    <t>$C$14</t>
+  </si>
+  <si>
+    <t>$C$4</t>
+  </si>
+  <si>
+    <t>Contin</t>
+  </si>
+  <si>
+    <t>$C$5</t>
+  </si>
+  <si>
+    <t>$C$14=640000</t>
+  </si>
+  <si>
+    <t>Binding</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Sensitivity Report</t>
+  </si>
+  <si>
+    <t>Report Created: Mar 26, 2025 2:37:22 PM</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Reduced</t>
+  </si>
+  <si>
+    <t>Gradient</t>
+  </si>
+  <si>
+    <t>Lagrange</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Limits Report</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Limit</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Upper</t>
+  </si>
+  <si>
+    <t>Report Created: Mar 26, 2025 2:44:21 PM</t>
+  </si>
+  <si>
+    <t>Solution Time: 0.062 Seconds.</t>
+  </si>
+  <si>
+    <t>Iterations: 2 Subproblems: 0</t>
+  </si>
+  <si>
+    <t>$C$4&lt;=0.2</t>
+  </si>
+  <si>
+    <t>Not Binding</t>
+  </si>
+  <si>
+    <t>$C$5&lt;=0.05</t>
   </si>
 </sst>
 </file>
@@ -138,13 +359,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,16 +396,91 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="9"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="18"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="20"/>
+        <bgColor indexed="24"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="24"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -370,6 +666,64 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -378,19 +732,187 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -411,32 +933,126 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="14" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="14" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="15" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -13757,7 +14373,7 @@
         <v>66.716957191670204</v>
       </c>
       <c r="D399" s="10">
-        <f t="shared" ref="D399:D430" si="4">C399-_xlfn.FORECAST.ETS.CONFINT(A399,$B$2:$B$366,$A$2:$A$366,0.95,1,1)</f>
+        <f t="shared" ref="D399:D427" si="4">C399-_xlfn.FORECAST.ETS.CONFINT(A399,$B$2:$B$366,$A$2:$A$366,0.95,1,1)</f>
         <v>-27.387538454538941</v>
       </c>
       <c r="E399" s="10">
@@ -14251,38 +14867,1068 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F2C323-B90C-465D-8DE6-80FFB8C5DA34}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37317632-790B-451A-A5DB-9C8069A906AC}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="B1:G18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="12.6640625" bestFit="1" customWidth="1" outlineLevel="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="48"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+    </row>
+    <row r="3" spans="2:7" ht="15.6" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="32.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="58" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="51"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+    </row>
+    <row r="6" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="50"/>
+      <c r="C6" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="43">
+        <v>100000</v>
+      </c>
+      <c r="E6" s="55">
+        <v>100000</v>
+      </c>
+      <c r="F6" s="55">
+        <v>80000</v>
+      </c>
+      <c r="G6" s="55">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="50"/>
+      <c r="C7" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="56">
+        <v>0.15</v>
+      </c>
+      <c r="G7" s="56">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="50"/>
+      <c r="C8" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="45">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E8" s="57">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F8" s="57">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G8" s="57">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="51"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+    </row>
+    <row r="10" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="50"/>
+      <c r="C10" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="43">
+        <v>110000</v>
+      </c>
+      <c r="E10" s="43">
+        <v>110000</v>
+      </c>
+      <c r="F10" s="43">
+        <v>110000</v>
+      </c>
+      <c r="G10" s="43">
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="50"/>
+      <c r="C11" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="43">
+        <v>111650</v>
+      </c>
+      <c r="E11" s="43">
+        <v>111650</v>
+      </c>
+      <c r="F11" s="43">
+        <v>111650</v>
+      </c>
+      <c r="G11" s="43">
+        <v>111650</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="50"/>
+      <c r="C12" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="43">
+        <v>113324.75</v>
+      </c>
+      <c r="E12" s="43">
+        <v>113324.75</v>
+      </c>
+      <c r="F12" s="43">
+        <v>113324.75</v>
+      </c>
+      <c r="G12" s="43">
+        <v>113324.75</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="50"/>
+      <c r="C13" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="43">
+        <v>115024.62125</v>
+      </c>
+      <c r="E13" s="43">
+        <v>115024.62125</v>
+      </c>
+      <c r="F13" s="43">
+        <v>115024.62125</v>
+      </c>
+      <c r="G13" s="43">
+        <v>115024.62125</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="50"/>
+      <c r="C14" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="43">
+        <v>116749.99056875</v>
+      </c>
+      <c r="E14" s="43">
+        <v>116749.99056875</v>
+      </c>
+      <c r="F14" s="43">
+        <v>116749.99056875</v>
+      </c>
+      <c r="G14" s="43">
+        <v>116749.99056875</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="52"/>
+      <c r="C15" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="46">
+        <v>566749.36181875004</v>
+      </c>
+      <c r="E15" s="46">
+        <v>566749.36181875004</v>
+      </c>
+      <c r="F15" s="46">
+        <v>566749.36181875004</v>
+      </c>
+      <c r="G15" s="46">
+        <v>566749.36181875004</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9789B918-84CC-4151-AE9D-7D2E8DEB9462}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" collapsed="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="60" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="62">
+        <v>566749.36179999996</v>
+      </c>
+      <c r="E16" s="62">
+        <v>639999.95109999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="60" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="63">
+        <v>0.1</v>
+      </c>
+      <c r="E21" s="63">
+        <v>0.226693026881682</v>
+      </c>
+      <c r="F21" s="61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="64">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E22" s="64">
+        <v>2.1270607913771021E-2</v>
+      </c>
+      <c r="F22" s="59" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="62">
+        <v>639999.94999999995</v>
+      </c>
+      <c r="E27" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" s="59">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EFCC5C-41B8-46D5-84D8-EA5738816026}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="61">
+        <v>0.226693026881682</v>
+      </c>
+      <c r="E9" s="61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="59">
+        <v>2.1270607913771021E-2</v>
+      </c>
+      <c r="E10" s="59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="65" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="66" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="67">
+        <v>639999.94999999995</v>
+      </c>
+      <c r="E15" s="59">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9500024-5967-493D-8ABD-61719E0CAC04}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="65"/>
+      <c r="C6" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="65"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="66" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="62">
+        <v>639999.95109999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="65"/>
+      <c r="C11" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="65"/>
+      <c r="F11" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="65" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12" s="66" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="63">
+        <v>0.226693026881682</v>
+      </c>
+      <c r="F13" s="63">
+        <v>0</v>
+      </c>
+      <c r="G13" s="63">
+        <v>521727.88</v>
+      </c>
+      <c r="I13" s="61" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J13" s="61" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="64">
+        <v>2.1270607913771021E-2</v>
+      </c>
+      <c r="F14" s="64">
+        <v>0</v>
+      </c>
+      <c r="G14" s="64">
+        <v>613346.51</v>
+      </c>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98E50DE-0C1C-4869-BA2F-BF9F71F89025}">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" collapsed="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="60" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="62">
+        <v>622877.09439999994</v>
+      </c>
+      <c r="E16" s="62">
+        <v>640000.14520000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="60" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="63">
+        <v>0.15</v>
+      </c>
+      <c r="E21" s="63">
+        <v>0.17283479610661426</v>
+      </c>
+      <c r="F21" s="61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="64">
+        <v>0.04</v>
+      </c>
+      <c r="E22" s="64">
+        <v>4.3731865887940702E-2</v>
+      </c>
+      <c r="F22" s="59" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="68">
+        <v>640000.15</v>
+      </c>
+      <c r="E27" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" s="61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="63">
+        <v>0.17283479610661426</v>
+      </c>
+      <c r="E28" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="G28" s="61">
+        <v>2.7165203893385753E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="64">
+        <v>4.3731865887940702E-2</v>
+      </c>
+      <c r="E29" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="G29" s="59">
+        <v>6.2681341120593009E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{324DEB92-0BCB-43D5-9832-7695D02DB378}">
   <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="E2" s="19" t="s">
+      <c r="C2" s="16"/>
+      <c r="E2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="19" t="s">
         <v>8</v>
       </c>
     </row>
@@ -14290,10 +15936,10 @@
       <c r="B3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="20">
         <v>100000</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="21" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="22">
@@ -14302,7 +15948,7 @@
       <c r="G3" s="23">
         <v>0.1</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="24">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
@@ -14310,10 +15956,10 @@
       <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="E4" s="16" t="s">
+      <c r="C4" s="25">
+        <v>0.17283479610661426</v>
+      </c>
+      <c r="E4" s="21" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="22">
@@ -14322,7 +15968,7 @@
       <c r="G4" s="23">
         <v>0.15</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="24">
         <v>1.2E-2</v>
       </c>
     </row>
@@ -14330,78 +15976,126 @@
       <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="28">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E5" s="16" t="s">
+      <c r="C5" s="26">
+        <v>4.3731865887940702E-2</v>
+      </c>
+      <c r="E5" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="28">
         <v>120000</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="29">
         <v>0.05</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="30">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E6" s="17" t="s">
+    <row r="6" spans="2:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E6" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="18" t="e">
+      <c r="F6" s="32" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="33">
         <v>0.25</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="34">
         <v>0.04</v>
       </c>
     </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="16"/>
+    </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9">
+      <c r="B9" s="37">
         <v>0</v>
       </c>
+      <c r="C9" s="13">
+        <f>(base*(1+raise)^B9)*(1+bonus)</f>
+        <v>117283.47961066144</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10">
+      <c r="B10" s="37">
         <v>1</v>
       </c>
+      <c r="C10" s="13">
+        <f>(base*(1+raise)^B10)*(1+bonus)</f>
+        <v>122412.5050118659</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11">
+      <c r="B11" s="37">
         <v>2</v>
       </c>
+      <c r="C11" s="13">
+        <f>(base*(1+raise)^B11)*(1+bonus)</f>
+        <v>127765.83226405167</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12">
+      <c r="B12" s="37">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13">
+      <c r="C12" s="13">
+        <f>(base*(1+raise)^B12)*(1+bonus)</f>
+        <v>133353.27050568431</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="38">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="C13" s="39">
+        <f>(base*(1+raise)^B13)*(1+bonus)</f>
+        <v>139185.05784715715</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="40" t="s">
         <v>15</v>
       </c>
+      <c r="C14" s="41">
+        <f>SUM(C9:C13)</f>
+        <v>640000.14523942047</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <scenarios current="0" sqref="C9:C14">
+    <scenario name="Job 1" locked="1" count="3" user="Raph Adam" comment="Created by Raph Adam on 03 26 2025">
+      <inputCells r="C3" val="100000" numFmtId="165"/>
+      <inputCells r="C4" val="0.1" numFmtId="9"/>
+      <inputCells r="C5" val="0.015" numFmtId="167"/>
+    </scenario>
+    <scenario name="Job 2" locked="1" count="3" user="Raph Adam" comment="Created by Raph Adam on 03 26 2025">
+      <inputCells r="C3" val="80000" numFmtId="165"/>
+      <inputCells r="C4" val="0.15" numFmtId="9"/>
+      <inputCells r="C5" val="0.012" numFmtId="167"/>
+    </scenario>
+    <scenario name="Job 3" locked="1" count="3" user="Raph Adam" comment="Created by Raph Adam on 03 26 2025">
+      <inputCells r="C3" val="120000" numFmtId="165"/>
+      <inputCells r="C4" val="0.05" numFmtId="9"/>
+      <inputCells r="C5" val="0.008" numFmtId="167"/>
+    </scenario>
+  </scenarios>
+  <mergeCells count="2">
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>